<commit_message>
Basic items working. settings worked out.
</commit_message>
<xml_diff>
--- a/Pivot Table Option 1.xlsx
+++ b/Pivot Table Option 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffs\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Programming\VisualStudioProjects\TestConsoleApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4EC1B01-1A7E-4673-A588-2211F5A10997}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCEAD11-BE4C-4495-AD4D-25BA7C65FA3D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="11175" xr2:uid="{C1DBE9DF-368E-4014-A63D-02285EDA6258}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId2"/>
+    <pivotCache cacheId="6" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -286,7 +286,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jeff Stuyvesant" refreshedDate="43233.976778240743" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="24" xr:uid="{97736671-08FF-4619-8BFC-910B304C7C06}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jeff Stuyvesant" refreshedDate="43287.970120138889" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="24" xr:uid="{97736671-08FF-4619-8BFC-910B304C7C06}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B1:G25" sheet="Revisions"/>
   </cacheSource>
@@ -556,7 +556,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{65E0132C-41C8-4DA1-8C75-B81582BD7134}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{65E0132C-41C8-4DA1-8C75-B81582BD7134}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="L1:O31" firstHeaderRow="1" firstDataRow="1" firstDataCol="4"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -1049,7 +1049,7 @@
   <dimension ref="A1:Z30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>